<commit_message>
Added PR pipeline-comparison notebook
</commit_message>
<xml_diff>
--- a/data/2023-10-24_pr-dna/virus-counts-pr.xlsx
+++ b/data/2023-10-24_pr-dna/virus-counts-pr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will2/Dropbox/dev/work/wills-public-notebook/data/2023-10-24_pr-dna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F5EEB9F-6DCB-8C47-A7A3-AC3BA6CE562E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A4E3E1-A06D-6F48-BC74-E3204A382071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19200" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{7E1414A2-310C-D844-88DC-A2DCC9D18744}"/>
+    <workbookView xWindow="3460" yWindow="3540" windowWidth="15020" windowHeight="12440" xr2:uid="{7E1414A2-310C-D844-88DC-A2DCC9D18744}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -422,7 +422,7 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>